<commit_message>
percentages:: by sergio giraldo @ 20230305T1941CET, gpg signed
</commit_message>
<xml_diff>
--- a/excel/match-offset-index.xlsx
+++ b/excel/match-offset-index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F22696-295B-DD48-9422-4D55B899156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F9CC2A-D83B-834C-B6A2-DF66D8969B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{89C61F2D-2644-0A4E-AA27-51E05C734111}"/>
   </bookViews>
@@ -206,15 +206,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -222,15 +228,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +581,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,96 +750,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C5AE20-61FF-9442-95EF-18BC216E5DC7}">
-  <dimension ref="A1:AA32"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" style="5" customWidth="1"/>
+    <col min="2" max="27" width="4.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3">
@@ -889,7 +927,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3">
@@ -972,7 +1010,7 @@
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3">
@@ -1055,7 +1093,7 @@
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3">
@@ -1138,7 +1176,7 @@
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
@@ -1221,7 +1259,7 @@
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3">
@@ -1304,7 +1342,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3">
@@ -1387,7 +1425,7 @@
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3">
@@ -1470,7 +1508,7 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3">
@@ -1553,7 +1591,7 @@
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3">
@@ -1636,7 +1674,7 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3">
@@ -1719,7 +1757,7 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3">
@@ -1802,7 +1840,7 @@
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="3">
@@ -1885,7 +1923,7 @@
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="3">
@@ -1968,7 +2006,7 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="3">
@@ -2051,7 +2089,7 @@
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3">
@@ -2134,7 +2172,7 @@
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3">
@@ -2217,7 +2255,7 @@
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="3">
@@ -2300,7 +2338,7 @@
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3">
@@ -2383,7 +2421,7 @@
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="3">
@@ -2466,7 +2504,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="3">
@@ -2549,7 +2587,7 @@
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="3">
@@ -2632,7 +2670,7 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="3">
@@ -2715,7 +2753,7 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="3">
@@ -2798,7 +2836,7 @@
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="3">
@@ -2881,7 +2919,7 @@
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="3">
@@ -2961,12 +2999,6 @@
       </c>
       <c r="AA27" s="3">
         <v>798</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="F32">
-        <f ca="1">OFFSET(A1,19,8)</f>
-        <v>556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>